<commit_message>
finalizado so  falta responder a perg
</commit_message>
<xml_diff>
--- a/Chuteira_Puma.xlsx
+++ b/Chuteira_Puma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\OneDrive\Documentos\Ciencia dos dados\Projeto1_CD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103FED2C-95EA-48B2-B943-23745CA62829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AAE7E8-1A13-440F-AF76-77A3073CBFBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="604">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1888,6 +1888,9 @@
   </si>
   <si>
     <t>Irrelevante</t>
+  </si>
+  <si>
+    <t>classificacao</t>
   </si>
 </sst>
 </file>
@@ -1911,7 +1914,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1939,6 +1942,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1970,7 +1985,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1984,7 +1999,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2330,7 +2350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3565,16 +3585,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C160"/>
+  <dimension ref="A1:C300"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="D168" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="165.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="255.77734375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3582,1227 +3604,2401 @@
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>602</v>
-      </c>
+      <c r="B1" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B4" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B5" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B6" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B7" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B8" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B9" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B11" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B12" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B16" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B17" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B18" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="B19" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B20" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B21" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B22" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B23" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="B24" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B25" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B26" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B27" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B28" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B29" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="B30" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B31" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B32" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B33" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="B34" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="B35" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="B36" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B37" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B38" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="B39" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="B40" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B41" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B42" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B43" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B44" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="B45" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="B46" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B47" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B48" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B49" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B50" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B51" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B52" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="B53" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="B54" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="B55" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="B56" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B57" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="B58" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B59" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="B60" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="B61" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="B62" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="B63" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="B64" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="B65" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="B66" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="B67" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="B68" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="B69" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B70" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="B71" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B72" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="B73" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="B74" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="B75" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="B76" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="B77" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="B78" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B79" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="B80" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="B81" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="B82" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="B83" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="B84" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="B85" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="B86" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="B87" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B88" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B89" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="B90" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="B91" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="B92" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="B93" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B94" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="B95" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="B96" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="B97" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="B98" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="B99" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="B100" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="B101" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="B102" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="B103" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B104" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="B105" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="B106" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="B107" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B108" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="B109" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="B110" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="B111" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="B112" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="B113" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="B114" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="B115" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="B116" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="B117" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B118" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="B119" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="B120" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="B121" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="B122" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="B123" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="B124" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="B125" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="B126" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="B127" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="B128" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="B129" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="B130" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="B131" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B132" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="B133" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="B134" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="B135" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="B136" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="B137" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="B138" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="B139" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B140" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B141" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="5" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B142" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="5" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B143" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="5" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B144" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="5" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B145" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="5" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B146" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="5" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="B147" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="5" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B148" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="5" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B149" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" s="5" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B150" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="5" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B151" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" s="5" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="B152" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="5" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="B153" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" s="5" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="B154" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" s="5" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="B155" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" s="5" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B156" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" s="5" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B157" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" s="5" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B158" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" s="5" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="B159" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" s="5" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="B160" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" s="5" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="B161" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" s="5" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="B162" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" s="5" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="B163" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" s="5" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="B164" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" s="5" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="B165" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" s="5" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="B166" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" s="5" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B28" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="B167" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" s="5" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B29" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="B168" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" s="5" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="B169" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" s="5" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B31" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="B170" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" s="5" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="B171" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" s="5" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="C33" s="5" t="s">
+      <c r="B172" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" s="5" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="B173" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" s="5" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="B174" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" s="5" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="B175" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" s="5" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="B176" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" s="5" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="B177" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" s="5" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="B178" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" s="5" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="B179" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" s="5" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="B180" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" s="5" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="C42" s="5" t="s">
+      <c r="B181" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" s="5" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="C43" s="5" t="s">
+      <c r="B182" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" s="5" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="B183" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" s="5" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="B184" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185" s="5" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="C46" s="5" t="s">
+      <c r="B185" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186" s="5" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="C47" s="5" t="s">
+      <c r="B186" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187" s="5" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B48" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="C48" s="5" t="s">
+      <c r="B187" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188" s="5" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B49" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="C49" s="5" t="s">
+      <c r="B188" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189" s="5" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" s="4" t="s">
-        <v>423</v>
-      </c>
-      <c r="C50" s="5" t="s">
+      <c r="B189" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190" s="5" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B51" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="C51" s="5" t="s">
+      <c r="B190" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191" s="5" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B52" s="4" t="s">
-        <v>426</v>
-      </c>
-      <c r="C52" s="5" t="s">
+      <c r="B191" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192" s="5" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="C53" s="5" t="s">
+      <c r="B192" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193" s="5" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B54" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="C54" s="5" t="s">
+      <c r="B193" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A194" s="5" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B55" s="4" t="s">
-        <v>431</v>
-      </c>
-      <c r="C55" s="5" t="s">
+      <c r="B194" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195" s="5" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B56" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="C56" s="5" t="s">
+      <c r="B195" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196" s="5" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="C57" s="5" t="s">
+      <c r="B196" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197" s="5" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B58" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="C58" s="5" t="s">
+      <c r="B197" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198" s="5" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B59" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="C59" s="5" t="s">
+      <c r="B198" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199" s="5" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="C60" s="5" t="s">
+      <c r="B199" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200" s="5" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="C61" s="5" t="s">
+      <c r="B200" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201" s="5" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B62" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="C62" s="5" t="s">
+      <c r="B201" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202" s="5" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B63" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="C63" s="5" t="s">
+      <c r="B202" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A203" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B64" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="C64" s="5" t="s">
+      <c r="B203" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A204" s="5" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B65" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="C65" s="5" t="s">
+      <c r="B204" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A205" s="5" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B66" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="C66" s="5" t="s">
+      <c r="B205" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A206" s="5" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B67" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="C67" s="5" t="s">
+      <c r="B206" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207" s="5" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B68" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="C68" s="5" t="s">
+      <c r="B207" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" s="5" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B69" s="4" t="s">
-        <v>460</v>
-      </c>
-      <c r="C69" s="5" t="s">
+      <c r="B208" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A209" s="5" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="C70" s="5" t="s">
+      <c r="B209" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210" s="5" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B71" s="4" t="s">
-        <v>462</v>
-      </c>
-      <c r="C71" s="5" t="s">
+      <c r="B210" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A211" s="5" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B72" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="C72" s="5" t="s">
+      <c r="B211" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A212" s="5" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B73" s="4" t="s">
-        <v>464</v>
-      </c>
-      <c r="C73" s="5" t="s">
+      <c r="B212" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213" s="5" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B74" s="4" t="s">
-        <v>468</v>
-      </c>
-      <c r="C74" s="5" t="s">
+      <c r="B213" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214" s="5" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B75" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="C75" s="5" t="s">
+      <c r="B214" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A215" s="5" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B76" s="4" t="s">
-        <v>470</v>
-      </c>
-      <c r="C76" s="5" t="s">
+      <c r="B215" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216" s="5" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B77" s="4" t="s">
-        <v>471</v>
-      </c>
-      <c r="C77" s="5" t="s">
+      <c r="B216" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A217" s="5" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B78" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="C78" s="5" t="s">
+      <c r="B217" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A218" s="5" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B79" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="C79" s="5" t="s">
+      <c r="B218" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A219" s="5" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B80" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="C80" s="5" t="s">
+      <c r="B219" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A220" s="5" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B81" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="C81" s="5" t="s">
+      <c r="B220" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A221" s="5" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B82" s="4" t="s">
-        <v>485</v>
-      </c>
-      <c r="C82" s="5" t="s">
+      <c r="B221" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222" s="5" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B83" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="C83" s="5" t="s">
+      <c r="B222" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" s="5" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B84" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="C84" s="5" t="s">
+      <c r="B223" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A224" s="5" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B85" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="C85" s="5" t="s">
+      <c r="B224" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" s="5" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B86" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="C86" s="5" t="s">
+      <c r="B225" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" s="5" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B87" s="4" t="s">
-        <v>495</v>
-      </c>
-      <c r="C87" s="5" t="s">
+      <c r="B226" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227" s="5" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B88" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="C88" s="5" t="s">
+      <c r="B227" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A228" s="5" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B89" s="4" t="s">
-        <v>498</v>
-      </c>
-      <c r="C89" s="5" t="s">
+      <c r="B228" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A229" s="5" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B90" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="C90" s="5" t="s">
+      <c r="B229" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A230" s="5" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B91" s="4" t="s">
-        <v>508</v>
-      </c>
-      <c r="C91" s="5" t="s">
+      <c r="B230" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A231" s="5" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B92" s="4" t="s">
-        <v>509</v>
-      </c>
-      <c r="C92" s="5" t="s">
+      <c r="B231" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A232" s="5" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B93" s="4" t="s">
-        <v>510</v>
-      </c>
-      <c r="C93" s="5" t="s">
+      <c r="B232" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A233" s="5" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B94" s="4" t="s">
-        <v>511</v>
-      </c>
-      <c r="C94" s="5" t="s">
+      <c r="B233" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A234" s="5" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B95" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="C95" s="5" t="s">
+      <c r="B234" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A235" s="5" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B96" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="C96" s="5" t="s">
+      <c r="B235" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A236" s="5" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B97" s="4" t="s">
-        <v>519</v>
-      </c>
-      <c r="C97" s="5" t="s">
+      <c r="B236" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A237" s="5" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B98" s="4" t="s">
-        <v>522</v>
-      </c>
-      <c r="C98" s="5" t="s">
+      <c r="B237" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A238" s="5" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B99" s="4" t="s">
-        <v>523</v>
-      </c>
-      <c r="C99" s="5" t="s">
+      <c r="B238" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A239" s="5" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B100" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="C100" s="5" t="s">
+      <c r="B239" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A240" s="5" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B101" s="4" t="s">
-        <v>530</v>
-      </c>
-      <c r="C101" s="5" t="s">
+      <c r="B240" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A241" s="5" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B102" s="4" t="s">
-        <v>531</v>
-      </c>
-      <c r="C102" s="5" t="s">
+      <c r="B241" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A242" s="5" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B103" s="4" t="s">
-        <v>532</v>
-      </c>
-      <c r="C103" s="5" t="s">
+      <c r="B242" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A243" s="5" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B104" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="C104" s="5" t="s">
+      <c r="B243" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A244" s="5" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B105" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="C105" s="5" t="s">
+      <c r="B244" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A245" s="5" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B106" s="4" t="s">
-        <v>537</v>
-      </c>
-      <c r="C106" s="5" t="s">
+      <c r="B245" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A246" s="5" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B107" s="4" t="s">
-        <v>539</v>
-      </c>
-      <c r="C107" s="5" t="s">
+      <c r="B246" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A247" s="5" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B108" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="C108" s="5" t="s">
+      <c r="B247" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A248" s="5" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B109" s="4" t="s">
-        <v>541</v>
-      </c>
-      <c r="C109" s="5" t="s">
+      <c r="B248" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A249" s="5" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B110" s="4" t="s">
-        <v>542</v>
-      </c>
-      <c r="C110" s="5" t="s">
+      <c r="B249" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A250" s="5" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B111" s="4" t="s">
-        <v>599</v>
-      </c>
-      <c r="C111" s="5" t="s">
+      <c r="B250" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A251" s="5" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B112" s="4" t="s">
-        <v>551</v>
-      </c>
-      <c r="C112" s="5" t="s">
+      <c r="B251" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A252" s="5" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B113" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="C113" s="5" t="s">
+      <c r="B252" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A253" s="5" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B114" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="C114" s="5" t="s">
+      <c r="B253" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A254" s="5" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B115" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="C115" s="5" t="s">
+      <c r="B254" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A255" s="5" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B116" s="4" t="s">
-        <v>560</v>
-      </c>
-      <c r="C116" s="5" t="s">
+      <c r="B255" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A256" s="5" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B117" s="4" t="s">
-        <v>598</v>
-      </c>
-      <c r="C117" s="5" t="s">
+      <c r="B256" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A257" s="5" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B118" s="4" t="s">
-        <v>561</v>
-      </c>
-      <c r="C118" s="5" t="s">
+      <c r="B257" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A258" s="5" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B119" s="4" t="s">
-        <v>567</v>
-      </c>
-      <c r="C119" s="5" t="s">
+      <c r="B258" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A259" s="5" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B120" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="C120" s="5" t="s">
+      <c r="B259" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A260" s="5" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B121" s="4" t="s">
-        <v>585</v>
-      </c>
-      <c r="C121" s="5" t="s">
+      <c r="B260" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A261" s="5" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B122" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="C122" s="5" t="s">
+      <c r="B261" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A262" s="5" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B123" s="4" t="s">
-        <v>563</v>
-      </c>
-      <c r="C123" s="5" t="s">
+      <c r="B262" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A263" s="5" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B124" s="4" t="s">
-        <v>594</v>
-      </c>
-      <c r="C124" s="5" t="s">
+      <c r="B263" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A264" s="5" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B125" s="4" t="s">
-        <v>586</v>
-      </c>
-      <c r="C125" s="5" t="s">
+      <c r="B264" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265" s="5" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B126" s="4" t="s">
-        <v>600</v>
-      </c>
-      <c r="C126" s="5" t="s">
+      <c r="B265" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A266" s="5" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B127" s="4" t="s">
-        <v>559</v>
-      </c>
-      <c r="C127" s="5" t="s">
+      <c r="B266" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A267" s="5" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B128" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="C128" s="5" t="s">
+      <c r="B267" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A268" s="5" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B129" s="4" t="s">
-        <v>552</v>
-      </c>
-      <c r="C129" s="5" t="s">
+      <c r="B268" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A269" s="5" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B130" s="4" t="s">
-        <v>569</v>
-      </c>
-      <c r="C130" s="5" t="s">
+      <c r="B269" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A270" s="5" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B131" s="4" t="s">
-        <v>543</v>
-      </c>
-      <c r="C131" s="5" t="s">
+      <c r="B270" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A271" s="5" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B132" s="4" t="s">
-        <v>564</v>
-      </c>
-      <c r="C132" s="5" t="s">
+      <c r="B271" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A272" s="5" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B133" s="4" t="s">
-        <v>593</v>
-      </c>
-      <c r="C133" s="5" t="s">
+      <c r="B272" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A273" s="5" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B134" s="4" t="s">
-        <v>578</v>
-      </c>
-      <c r="C134" s="5" t="s">
+      <c r="B273" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A274" s="5" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B135" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="C135" s="5" t="s">
+      <c r="B274" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A275" s="5" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B136" s="4" t="s">
-        <v>565</v>
-      </c>
-      <c r="C136" s="5" t="s">
+      <c r="B275" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A276" s="5" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B137" s="4" t="s">
-        <v>597</v>
-      </c>
-      <c r="C137" s="5" t="s">
+      <c r="B276" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A277" s="5" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B138" s="4" t="s">
-        <v>579</v>
-      </c>
-      <c r="C138" s="5" t="s">
+      <c r="B277" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A278" s="5" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B139" s="4" t="s">
-        <v>591</v>
-      </c>
-      <c r="C139" s="5" t="s">
+      <c r="B278" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A279" s="5" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B140" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="C140" s="5" t="s">
+      <c r="B279" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A280" s="5" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B141" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="C141" s="5" t="s">
+      <c r="B280" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A281" s="5" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C142" s="5" t="s">
+      <c r="B281" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A282" s="5" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C143" s="5" t="s">
+      <c r="B282" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A283" s="5" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C144" s="5" t="s">
+      <c r="B283" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A284" s="5" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C145" s="5" t="s">
+      <c r="B284" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A285" s="5" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C146" s="5" t="s">
+      <c r="B285" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A286" s="5" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C147" s="5" t="s">
+      <c r="B286" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A287" s="5" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C148" s="5" t="s">
+      <c r="B287" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A288" s="5" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C149" s="5" t="s">
+      <c r="B288" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A289" s="5" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C150" s="5" t="s">
+      <c r="B289" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A290" s="5" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C151" s="5" t="s">
+      <c r="B290" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A291" s="5" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C152" s="5" t="s">
+      <c r="B291" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A292" s="5" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C153" s="5" t="s">
+      <c r="B292" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A293" s="5" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C154" s="5" t="s">
+      <c r="B293" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A294" s="5" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C155" s="5" t="s">
+      <c r="B294" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A295" s="5" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C156" s="5" t="s">
+      <c r="B295" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A296" s="5" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="157" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C157" s="5" t="s">
+      <c r="B296" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A297" s="5" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="158" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C158" s="5" t="s">
+      <c r="B297" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A298" s="5" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C159" s="5" t="s">
+      <c r="B298" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A299" s="5" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C160" s="6" t="s">
+      <c r="B299" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A300" s="6" t="s">
         <v>590</v>
+      </c>
+      <c r="B300" t="s">
+        <v>602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>